<commit_message>
test: update test outputs
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_test_excluded_composition.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_test_excluded_composition.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,20 +12,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>numeric system score</t>
-  </si>
-  <si>
-    <t>non-numeric system score</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64,22 +50,89 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -380,23 +433,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>numeric system score</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>non-numeric system score</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3">
       <c r="A3" t="n">
         <v>0</v>
       </c>
@@ -404,7 +459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4">
       <c r="A4" t="n">
         <v>0</v>
       </c>
@@ -413,6 +468,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>